<commit_message>
Change highlighting in test cases
</commit_message>
<xml_diff>
--- a/docs/xlsx/test_cases.xlsx
+++ b/docs/xlsx/test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\wsw-results\docs\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FE6EFD-EC2C-4E54-BADE-7166C8D87FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E55A53-539B-4E67-9D2B-F8900DCC3E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="10" xr2:uid="{D7C2B3EB-C644-453F-9AFF-1FCF05F25229}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D7C2B3EB-C644-453F-9AFF-1FCF05F25229}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="1" r:id="rId1"/>
@@ -592,9 +592,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807B617B-7C45-4DFD-80F6-95980D161D4A}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,10 +635,10 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
@@ -1435,7 +1435,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,9 +1898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05E4C16-2D53-415C-8740-8D0C227F23E8}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2390,7 +2390,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2462,7 +2462,7 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
@@ -2478,7 +2478,7 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
@@ -2798,7 +2798,7 @@
       <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="2"/>
@@ -2812,7 +2812,7 @@
       <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D25" t="s">
@@ -2828,7 +2828,7 @@
       <c r="B26" t="s">
         <v>5</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D26" t="s">
@@ -2844,7 +2844,7 @@
       <c r="B27" t="s">
         <v>5</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D27" t="s">
@@ -2862,7 +2862,7 @@
       <c r="B28" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -3954,7 +3954,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -6366,7 +6366,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tweak highlighting in test cases
</commit_message>
<xml_diff>
--- a/docs/xlsx/test_cases.xlsx
+++ b/docs/xlsx/test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\wsw-results\docs\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E55A53-539B-4E67-9D2B-F8900DCC3E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD4EC80-5DF9-4424-974C-0B3BEEC09C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D7C2B3EB-C644-453F-9AFF-1FCF05F25229}"/>
   </bookViews>
@@ -594,7 +594,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +832,7 @@
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">

</xml_diff>